<commit_message>
remove unused package and modify import statements
trying to get API running again
</commit_message>
<xml_diff>
--- a/insider_transactions/insider_buying.xlsx
+++ b/insider_transactions/insider_buying.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="226">
   <si>
     <t>Ticker</t>
   </si>
@@ -70,6 +70,24 @@
     <t>A</t>
   </si>
   <si>
+    <t>AMCR</t>
+  </si>
+  <si>
+    <t>AAL</t>
+  </si>
+  <si>
+    <t>AXP</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>AWK</t>
+  </si>
+  <si>
+    <t>AMGN</t>
+  </si>
+  <si>
     <t>03/06/2023</t>
   </si>
   <si>
@@ -211,6 +229,54 @@
     <t>05/26/2021</t>
   </si>
   <si>
+    <t>04/06/2020</t>
+  </si>
+  <si>
+    <t>02/28/2020</t>
+  </si>
+  <si>
+    <t>02/24/2020</t>
+  </si>
+  <si>
+    <t>10/24/2023</t>
+  </si>
+  <si>
+    <t>11/08/2022</t>
+  </si>
+  <si>
+    <t>02/11/2020</t>
+  </si>
+  <si>
+    <t>06/28/2024</t>
+  </si>
+  <si>
+    <t>03/14/2024</t>
+  </si>
+  <si>
+    <t>10/30/2020</t>
+  </si>
+  <si>
+    <t>05/06/2020</t>
+  </si>
+  <si>
+    <t>08/28/2023</t>
+  </si>
+  <si>
+    <t>05/18/2023</t>
+  </si>
+  <si>
+    <t>05/02/2023</t>
+  </si>
+  <si>
+    <t>03/01/2021</t>
+  </si>
+  <si>
+    <t>05/13/2020</t>
+  </si>
+  <si>
+    <t>09/19/2023</t>
+  </si>
+  <si>
     <t>Michael M Larsen</t>
   </si>
   <si>
@@ -352,6 +418,42 @@
     <t>Ellen R Strahlman</t>
   </si>
   <si>
+    <t>Nicholas T. Long</t>
+  </si>
+  <si>
+    <t>MICHAEL J EMBLER</t>
+  </si>
+  <si>
+    <t>JOHN T CAHILL</t>
+  </si>
+  <si>
+    <t>Walter Joseph III Clayton</t>
+  </si>
+  <si>
+    <t>Lynn Ann Pike</t>
+  </si>
+  <si>
+    <t>John C Inglis</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL GROUP INC AMERICAN</t>
+  </si>
+  <si>
+    <t>WILLIAM G JURGENSEN</t>
+  </si>
+  <si>
+    <t>Michael Marberry</t>
+  </si>
+  <si>
+    <t>MARTHA CLARK GOSS</t>
+  </si>
+  <si>
+    <t>Lloyd M Yates</t>
+  </si>
+  <si>
+    <t>INC AMGEN</t>
+  </si>
+  <si>
     <t>$66.89</t>
   </si>
   <si>
@@ -536,6 +638,60 @@
   </si>
   <si>
     <t>$49.59</t>
+  </si>
+  <si>
+    <t>$8.20</t>
+  </si>
+  <si>
+    <t>$19.33</t>
+  </si>
+  <si>
+    <t>$18.96</t>
+  </si>
+  <si>
+    <t>$25.14</t>
+  </si>
+  <si>
+    <t>$143.93</t>
+  </si>
+  <si>
+    <t>$149.27</t>
+  </si>
+  <si>
+    <t>$132.87</t>
+  </si>
+  <si>
+    <t>$74.89</t>
+  </si>
+  <si>
+    <t>$75.39</t>
+  </si>
+  <si>
+    <t>$16.00</t>
+  </si>
+  <si>
+    <t>$24.10</t>
+  </si>
+  <si>
+    <t>$130.20</t>
+  </si>
+  <si>
+    <t>$141.07</t>
+  </si>
+  <si>
+    <t>$142.35</t>
+  </si>
+  <si>
+    <t>$145.89</t>
+  </si>
+  <si>
+    <t>$144.83</t>
+  </si>
+  <si>
+    <t>$115.95</t>
+  </si>
+  <si>
+    <t>$17.00</t>
   </si>
 </sst>
 </file>
@@ -893,7 +1049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -927,16 +1083,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>4000</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="F2">
         <v>267540</v>
@@ -950,16 +1106,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>3925</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="F3">
         <v>274239.75</v>
@@ -973,16 +1129,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>4000</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="F4">
         <v>267540</v>
@@ -996,16 +1152,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D5">
         <v>3925</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="F5">
         <v>274239.75</v>
@@ -1019,16 +1175,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D6">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="F6">
         <v>8505.380999999999</v>
@@ -1042,16 +1198,16 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D7">
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="F7">
         <v>19680</v>
@@ -1065,16 +1221,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="D8">
         <v>1200</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="F8">
         <v>336672</v>
@@ -1088,16 +1244,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>3250</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="F9">
         <v>936357.5</v>
@@ -1111,16 +1267,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="D10">
         <v>491</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F10">
         <v>250272.52</v>
@@ -1134,16 +1290,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D11">
         <v>2450</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="F11">
         <v>39935</v>
@@ -1157,16 +1313,16 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>2450</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="F12">
         <v>40106.5</v>
@@ -1180,16 +1336,16 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D13">
         <v>3000</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="F13">
         <v>49080</v>
@@ -1203,16 +1359,16 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D14">
         <v>1530</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="F14">
         <v>25092</v>
@@ -1226,16 +1382,16 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D15">
         <v>1529</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="F15">
         <v>25075.6</v>
@@ -1249,16 +1405,16 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <v>50000</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="F16">
         <v>819000</v>
@@ -1272,16 +1428,16 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D17">
         <v>27400</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="F17">
         <v>500598</v>
@@ -1295,16 +1451,16 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="D18">
         <v>1500</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="F18">
         <v>29265</v>
@@ -1318,16 +1474,16 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D19">
         <v>12000</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="F19">
         <v>233520</v>
@@ -1341,16 +1497,16 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D20">
         <v>47000</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="F20">
         <v>1001100</v>
@@ -1364,16 +1520,16 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D21">
         <v>5000</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="F21">
         <v>119025</v>
@@ -1387,16 +1543,16 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D22">
         <v>500000</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="F22">
         <v>6110000</v>
@@ -1410,16 +1566,16 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D23">
         <v>500000</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="F23">
         <v>5835000</v>
@@ -1433,16 +1589,16 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D24">
         <v>4300</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="F24">
         <v>48461</v>
@@ -1456,16 +1612,16 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D25">
         <v>5300</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="F25">
         <v>48317.45</v>
@@ -1479,16 +1635,16 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D26">
         <v>2500</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="F26">
         <v>23800</v>
@@ -1502,16 +1658,16 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D27">
         <v>3240</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="F27">
         <v>30067.2</v>
@@ -1525,16 +1681,16 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D28">
         <v>5230</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F28">
         <v>49685</v>
@@ -1548,16 +1704,16 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D29">
         <v>924</v>
       </c>
       <c r="E29" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F29">
         <v>9106.944</v>
@@ -1571,16 +1727,16 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D30">
         <v>3000</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F30">
         <v>28500</v>
@@ -1594,16 +1750,16 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D31">
         <v>2650</v>
       </c>
       <c r="E31" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F31">
         <v>25168.905</v>
@@ -1617,16 +1773,16 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="D32">
         <v>3000</v>
       </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F32">
         <v>28500</v>
@@ -1640,16 +1796,16 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D33">
         <v>9523</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F33">
         <v>90468.5</v>
@@ -1663,16 +1819,16 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="D34">
         <v>10000</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="F34">
         <v>129900</v>
@@ -1686,16 +1842,16 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D35">
         <v>500</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="F35">
         <v>38645</v>
@@ -1709,16 +1865,16 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D36">
         <v>1500</v>
       </c>
       <c r="E36" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="F36">
         <v>114000</v>
@@ -1732,16 +1888,16 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D37">
         <v>1000</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="F37">
         <v>59360</v>
@@ -1755,16 +1911,16 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D38">
         <v>500</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="F38">
         <v>27605</v>
@@ -1778,16 +1934,16 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D39">
         <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="F39">
         <v>2866.995</v>
@@ -1801,16 +1957,16 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D40">
         <v>500</v>
       </c>
       <c r="E40" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="F40">
         <v>19067.5</v>
@@ -1824,16 +1980,16 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D41">
         <v>25000</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="F41">
         <v>657340</v>
@@ -1844,16 +2000,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D42">
         <v>2.59</v>
       </c>
       <c r="E42" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="F42">
         <v>287.7231</v>
@@ -1864,16 +2020,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="B43" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D43">
         <v>11000</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="F43">
         <v>2908620</v>
@@ -1884,16 +2040,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D44">
         <v>10000</v>
       </c>
       <c r="E44" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="F44">
         <v>2523400</v>
@@ -1904,16 +2060,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D45">
         <v>1679</v>
       </c>
       <c r="E45" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="F45">
         <v>499939.04</v>
@@ -1924,16 +2080,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="B46" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D46">
         <v>1637</v>
       </c>
       <c r="E46" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="F46">
         <v>500281.933</v>
@@ -1947,16 +2103,16 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D47">
         <v>2450</v>
       </c>
       <c r="E47" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="F47">
         <v>39935</v>
@@ -1970,16 +2126,16 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D48">
         <v>2450</v>
       </c>
       <c r="E48" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="F48">
         <v>40106.5</v>
@@ -1993,16 +2149,16 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D49">
         <v>3000</v>
       </c>
       <c r="E49" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="F49">
         <v>49080</v>
@@ -2016,16 +2172,16 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D50">
         <v>1530</v>
       </c>
       <c r="E50" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="F50">
         <v>25092</v>
@@ -2039,16 +2195,16 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D51">
         <v>1529</v>
       </c>
       <c r="E51" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="F51">
         <v>25075.6</v>
@@ -2062,16 +2218,16 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D52">
         <v>50000</v>
       </c>
       <c r="E52" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="F52">
         <v>819000</v>
@@ -2085,16 +2241,16 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D53">
         <v>27400</v>
       </c>
       <c r="E53" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="F53">
         <v>500598</v>
@@ -2108,16 +2264,16 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="D54">
         <v>1500</v>
       </c>
       <c r="E54" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="F54">
         <v>29265</v>
@@ -2131,16 +2287,16 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D55">
         <v>12000</v>
       </c>
       <c r="E55" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="F55">
         <v>233520</v>
@@ -2154,16 +2310,16 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D56">
         <v>47000</v>
       </c>
       <c r="E56" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="F56">
         <v>1001100</v>
@@ -2177,16 +2333,16 @@
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D57">
         <v>5000</v>
       </c>
       <c r="E57" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="F57">
         <v>119025</v>
@@ -2200,16 +2356,16 @@
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D58">
         <v>500000</v>
       </c>
       <c r="E58" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="F58">
         <v>6110000</v>
@@ -2223,16 +2379,16 @@
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D59">
         <v>500000</v>
       </c>
       <c r="E59" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="F59">
         <v>5835000</v>
@@ -2246,16 +2402,16 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D60">
         <v>4300</v>
       </c>
       <c r="E60" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="F60">
         <v>48461</v>
@@ -2269,16 +2425,16 @@
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D61">
         <v>5300</v>
       </c>
       <c r="E61" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="F61">
         <v>48317.45</v>
@@ -2292,16 +2448,16 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C62" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D62">
         <v>2500</v>
       </c>
       <c r="E62" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="F62">
         <v>23800</v>
@@ -2315,16 +2471,16 @@
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D63">
         <v>3240</v>
       </c>
       <c r="E63" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="F63">
         <v>30067.2</v>
@@ -2338,16 +2494,16 @@
         <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D64">
         <v>5230</v>
       </c>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F64">
         <v>49685</v>
@@ -2361,16 +2517,16 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D65">
         <v>924</v>
       </c>
       <c r="E65" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F65">
         <v>9106.944</v>
@@ -2384,16 +2540,16 @@
         <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C66" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D66">
         <v>3000</v>
       </c>
       <c r="E66" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F66">
         <v>28500</v>
@@ -2407,16 +2563,16 @@
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D67">
         <v>2650</v>
       </c>
       <c r="E67" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F67">
         <v>25168.905</v>
@@ -2430,16 +2586,16 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="D68">
         <v>3000</v>
       </c>
       <c r="E68" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F68">
         <v>28500</v>
@@ -2453,16 +2609,16 @@
         <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C69" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D69">
         <v>9523</v>
       </c>
       <c r="E69" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F69">
         <v>90468.5</v>
@@ -2476,16 +2632,16 @@
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C70" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="D70">
         <v>10000</v>
       </c>
       <c r="E70" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="F70">
         <v>129900</v>
@@ -2499,16 +2655,16 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D71">
         <v>500</v>
       </c>
       <c r="E71" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="F71">
         <v>38645</v>
@@ -2522,16 +2678,16 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D72">
         <v>1500</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="F72">
         <v>114000</v>
@@ -2545,16 +2701,16 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D73">
         <v>1000</v>
       </c>
       <c r="E73" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="F73">
         <v>59360</v>
@@ -2568,16 +2724,16 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C74" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D74">
         <v>500</v>
       </c>
       <c r="E74" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="F74">
         <v>27605</v>
@@ -2591,16 +2747,16 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C75" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D75">
         <v>50</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="F75">
         <v>2866.995</v>
@@ -2614,16 +2770,16 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C76" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D76">
         <v>500</v>
       </c>
       <c r="E76" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="F76">
         <v>19067.5</v>
@@ -2637,16 +2793,16 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C77" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D77">
         <v>25000</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="F77">
         <v>657340</v>
@@ -2657,16 +2813,16 @@
     </row>
     <row r="78" spans="1:7">
       <c r="B78" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C78" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D78">
         <v>2.59</v>
       </c>
       <c r="E78" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="F78">
         <v>287.7231</v>
@@ -2677,16 +2833,16 @@
     </row>
     <row r="79" spans="1:7">
       <c r="B79" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C79" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D79">
         <v>11000</v>
       </c>
       <c r="E79" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="F79">
         <v>2908620</v>
@@ -2697,16 +2853,16 @@
     </row>
     <row r="80" spans="1:7">
       <c r="B80" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C80" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D80">
         <v>10000</v>
       </c>
       <c r="E80" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="F80">
         <v>2523400</v>
@@ -2717,16 +2873,16 @@
     </row>
     <row r="81" spans="1:7">
       <c r="B81" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C81" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D81">
         <v>1679</v>
       </c>
       <c r="E81" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="F81">
         <v>499939.04</v>
@@ -2737,16 +2893,16 @@
     </row>
     <row r="82" spans="1:7">
       <c r="B82" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C82" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D82">
         <v>1637</v>
       </c>
       <c r="E82" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="F82">
         <v>500281.933</v>
@@ -2760,16 +2916,16 @@
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D83">
         <v>2450</v>
       </c>
       <c r="E83" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="F83">
         <v>39935</v>
@@ -2783,16 +2939,16 @@
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C84" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D84">
         <v>2450</v>
       </c>
       <c r="E84" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="F84">
         <v>40106.5</v>
@@ -2806,16 +2962,16 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C85" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D85">
         <v>3000</v>
       </c>
       <c r="E85" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="F85">
         <v>49080</v>
@@ -2829,16 +2985,16 @@
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C86" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D86">
         <v>1530</v>
       </c>
       <c r="E86" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="F86">
         <v>25092</v>
@@ -2852,16 +3008,16 @@
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C87" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D87">
         <v>1529</v>
       </c>
       <c r="E87" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="F87">
         <v>25075.6</v>
@@ -2875,16 +3031,16 @@
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C88" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D88">
         <v>50000</v>
       </c>
       <c r="E88" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="F88">
         <v>819000</v>
@@ -2898,16 +3054,16 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D89">
         <v>27400</v>
       </c>
       <c r="E89" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="F89">
         <v>500598</v>
@@ -2921,16 +3077,16 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="D90">
         <v>1500</v>
       </c>
       <c r="E90" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="F90">
         <v>29265</v>
@@ -2944,16 +3100,16 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D91">
         <v>12000</v>
       </c>
       <c r="E91" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="F91">
         <v>233520</v>
@@ -2967,16 +3123,16 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C92" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D92">
         <v>47000</v>
       </c>
       <c r="E92" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="F92">
         <v>1001100</v>
@@ -2990,16 +3146,16 @@
         <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D93">
         <v>5000</v>
       </c>
       <c r="E93" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="F93">
         <v>119025</v>
@@ -3013,16 +3169,16 @@
         <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C94" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D94">
         <v>500000</v>
       </c>
       <c r="E94" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="F94">
         <v>6110000</v>
@@ -3036,16 +3192,16 @@
         <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C95" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D95">
         <v>500000</v>
       </c>
       <c r="E95" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="F95">
         <v>5835000</v>
@@ -3059,16 +3215,16 @@
         <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C96" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D96">
         <v>4300</v>
       </c>
       <c r="E96" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="F96">
         <v>48461</v>
@@ -3082,16 +3238,16 @@
         <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C97" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D97">
         <v>5300</v>
       </c>
       <c r="E97" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="F97">
         <v>48317.45</v>
@@ -3105,16 +3261,16 @@
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C98" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D98">
         <v>2500</v>
       </c>
       <c r="E98" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="F98">
         <v>23800</v>
@@ -3128,16 +3284,16 @@
         <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C99" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D99">
         <v>3240</v>
       </c>
       <c r="E99" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="F99">
         <v>30067.2</v>
@@ -3151,16 +3307,16 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C100" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D100">
         <v>5230</v>
       </c>
       <c r="E100" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F100">
         <v>49685</v>
@@ -3174,16 +3330,16 @@
         <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C101" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D101">
         <v>924</v>
       </c>
       <c r="E101" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F101">
         <v>9106.944</v>
@@ -3197,16 +3353,16 @@
         <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C102" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D102">
         <v>3000</v>
       </c>
       <c r="E102" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F102">
         <v>28500</v>
@@ -3220,16 +3376,16 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C103" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D103">
         <v>2650</v>
       </c>
       <c r="E103" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F103">
         <v>25168.905</v>
@@ -3243,16 +3399,16 @@
         <v>9</v>
       </c>
       <c r="B104" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C104" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="D104">
         <v>3000</v>
       </c>
       <c r="E104" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F104">
         <v>28500</v>
@@ -3266,16 +3422,16 @@
         <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C105" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D105">
         <v>9523</v>
       </c>
       <c r="E105" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="F105">
         <v>90468.5</v>
@@ -3289,16 +3445,16 @@
         <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C106" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="D106">
         <v>10000</v>
       </c>
       <c r="E106" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="F106">
         <v>129900</v>
@@ -3312,16 +3468,16 @@
         <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C107" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D107">
         <v>500</v>
       </c>
       <c r="E107" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="F107">
         <v>38645</v>
@@ -3335,16 +3491,16 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C108" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D108">
         <v>1500</v>
       </c>
       <c r="E108" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="F108">
         <v>114000</v>
@@ -3358,16 +3514,16 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C109" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D109">
         <v>1000</v>
       </c>
       <c r="E109" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="F109">
         <v>59360</v>
@@ -3381,16 +3537,16 @@
         <v>10</v>
       </c>
       <c r="B110" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C110" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D110">
         <v>500</v>
       </c>
       <c r="E110" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="F110">
         <v>27605</v>
@@ -3404,16 +3560,16 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C111" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D111">
         <v>50</v>
       </c>
       <c r="E111" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="F111">
         <v>2866.995</v>
@@ -3427,16 +3583,16 @@
         <v>10</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C112" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D112">
         <v>500</v>
       </c>
       <c r="E112" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="F112">
         <v>19067.5</v>
@@ -3450,16 +3606,16 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C113" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D113">
         <v>25000</v>
       </c>
       <c r="E113" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="F113">
         <v>657340</v>
@@ -3470,16 +3626,16 @@
     </row>
     <row r="114" spans="1:7">
       <c r="B114" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C114" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D114">
         <v>2.59</v>
       </c>
       <c r="E114" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="F114">
         <v>287.7231</v>
@@ -3490,16 +3646,16 @@
     </row>
     <row r="115" spans="1:7">
       <c r="B115" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C115" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D115">
         <v>11000</v>
       </c>
       <c r="E115" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="F115">
         <v>2908620</v>
@@ -3510,16 +3666,16 @@
     </row>
     <row r="116" spans="1:7">
       <c r="B116" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C116" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D116">
         <v>10000</v>
       </c>
       <c r="E116" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="F116">
         <v>2523400</v>
@@ -3530,16 +3686,16 @@
     </row>
     <row r="117" spans="1:7">
       <c r="B117" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C117" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D117">
         <v>1679</v>
       </c>
       <c r="E117" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="F117">
         <v>499939.04</v>
@@ -3550,16 +3706,16 @@
     </row>
     <row r="118" spans="1:7">
       <c r="B118" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C118" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D118">
         <v>1637</v>
       </c>
       <c r="E118" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="F118">
         <v>500281.933</v>
@@ -3570,16 +3726,16 @@
     </row>
     <row r="119" spans="1:7">
       <c r="B119" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C119" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D119">
         <v>2.59</v>
       </c>
       <c r="E119" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="F119">
         <v>287.7231</v>
@@ -3593,16 +3749,16 @@
         <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C120" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D120">
         <v>22000</v>
       </c>
       <c r="E120" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="F120">
         <v>2038960</v>
@@ -3616,16 +3772,16 @@
         <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C121" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D121">
         <v>1373</v>
       </c>
       <c r="E121" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="F121">
         <v>167313.78</v>
@@ -3639,16 +3795,16 @@
         <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C122" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="D122">
         <v>1260</v>
       </c>
       <c r="E122" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="F122">
         <v>246317.4</v>
@@ -3662,16 +3818,16 @@
         <v>12</v>
       </c>
       <c r="B123" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C123" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="D123">
         <v>5470</v>
       </c>
       <c r="E123" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="F123">
         <v>993570.7999999999</v>
@@ -3685,16 +3841,16 @@
         <v>12</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C124" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D124">
         <v>1373</v>
       </c>
       <c r="E124" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="F124">
         <v>249886</v>
@@ -3708,16 +3864,16 @@
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C125" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="D125">
         <v>5241</v>
       </c>
       <c r="E125" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="F125">
         <v>999982.8</v>
@@ -3731,16 +3887,16 @@
         <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C126" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="D126">
         <v>806</v>
       </c>
       <c r="E126" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="F126">
         <v>151334.56</v>
@@ -3751,16 +3907,16 @@
     </row>
     <row r="127" spans="1:7">
       <c r="B127" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C127" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D127">
         <v>2065000</v>
       </c>
       <c r="E127" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="F127">
         <v>2065000</v>
@@ -3771,16 +3927,16 @@
     </row>
     <row r="128" spans="1:7">
       <c r="B128" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C128" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D128">
         <v>43478</v>
       </c>
       <c r="E128" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="F128">
         <v>999994</v>
@@ -3794,16 +3950,16 @@
         <v>13</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C129" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D129">
         <v>5194</v>
       </c>
       <c r="E129" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="F129">
         <v>999845</v>
@@ -3817,16 +3973,16 @@
         <v>13</v>
       </c>
       <c r="B130" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C130" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D130">
         <v>5319</v>
       </c>
       <c r="E130" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="F130">
         <v>999972</v>
@@ -3840,16 +3996,16 @@
         <v>13</v>
       </c>
       <c r="B131" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C131" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D131">
         <v>7000</v>
       </c>
       <c r="E131" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="F131">
         <v>1996800.4</v>
@@ -3863,16 +4019,16 @@
         <v>13</v>
       </c>
       <c r="B132" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C132" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="D132">
         <v>587</v>
       </c>
       <c r="E132" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="F132">
         <v>200660.08</v>
@@ -3886,16 +4042,16 @@
         <v>13</v>
       </c>
       <c r="B133" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C133" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D133">
         <v>2928</v>
       </c>
       <c r="E133" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="F133">
         <v>999912</v>
@@ -3909,16 +4065,16 @@
         <v>13</v>
       </c>
       <c r="B134" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C134" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="D134">
         <v>500</v>
       </c>
       <c r="E134" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="F134">
         <v>96597.39999999999</v>
@@ -3932,16 +4088,16 @@
         <v>13</v>
       </c>
       <c r="B135" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C135" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D135">
         <v>1500</v>
       </c>
       <c r="E135" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="F135">
         <v>285385.05</v>
@@ -3955,16 +4111,16 @@
         <v>13</v>
       </c>
       <c r="B136" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C136" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D136">
         <v>10600</v>
       </c>
       <c r="E136" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="F136">
         <v>1998987.22</v>
@@ -3978,16 +4134,16 @@
         <v>13</v>
       </c>
       <c r="B137" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C137" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D137">
         <v>1000</v>
       </c>
       <c r="E137" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="F137">
         <v>264420</v>
@@ -4001,16 +4157,16 @@
         <v>13</v>
       </c>
       <c r="B138" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C138" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D138">
         <v>6700</v>
       </c>
       <c r="E138" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="F138">
         <v>1999842.13</v>
@@ -4021,16 +4177,16 @@
     </row>
     <row r="139" spans="1:7">
       <c r="B139" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C139" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D139">
         <v>2065000</v>
       </c>
       <c r="E139" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="F139">
         <v>2065000</v>
@@ -4041,16 +4197,16 @@
     </row>
     <row r="140" spans="1:7">
       <c r="B140" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C140" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D140">
         <v>43478</v>
       </c>
       <c r="E140" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="F140">
         <v>999994</v>
@@ -4064,16 +4220,16 @@
         <v>14</v>
       </c>
       <c r="B141" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C141" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D141">
         <v>2065000</v>
       </c>
       <c r="E141" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="F141">
         <v>2065000</v>
@@ -4087,16 +4243,16 @@
         <v>14</v>
       </c>
       <c r="B142" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C142" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D142">
         <v>43478</v>
       </c>
       <c r="E142" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="F142">
         <v>999994</v>
@@ -4110,16 +4266,16 @@
         <v>15</v>
       </c>
       <c r="B143" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C143" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="D143">
         <v>1100</v>
       </c>
       <c r="E143" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="F143">
         <v>53416</v>
@@ -4133,16 +4289,16 @@
         <v>15</v>
       </c>
       <c r="B144" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C144" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="D144">
         <v>500</v>
       </c>
       <c r="E144" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="F144">
         <v>24127.5</v>
@@ -4156,16 +4312,16 @@
         <v>15</v>
       </c>
       <c r="B145" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C145" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="D145">
         <v>1200</v>
       </c>
       <c r="E145" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="F145">
         <v>73200</v>
@@ -4179,16 +4335,16 @@
         <v>16</v>
       </c>
       <c r="B146" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C146" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D146">
         <v>1200</v>
       </c>
       <c r="E146" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="F146">
         <v>48599.39999999999</v>
@@ -4202,16 +4358,16 @@
         <v>16</v>
       </c>
       <c r="B147" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C147" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="D147">
         <v>1100</v>
       </c>
       <c r="E147" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="F147">
         <v>44625.46000000001</v>
@@ -4225,16 +4381,16 @@
         <v>16</v>
       </c>
       <c r="B148" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C148" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D148">
         <v>2000</v>
       </c>
       <c r="E148" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="F148">
         <v>99175.60000000001</v>
@@ -4248,22 +4404,436 @@
         <v>17</v>
       </c>
       <c r="B149" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C149" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D149">
         <v>2.59</v>
       </c>
       <c r="E149" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="F149">
         <v>287.7231</v>
       </c>
       <c r="G149">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>18</v>
+      </c>
+      <c r="B150" t="s">
+        <v>71</v>
+      </c>
+      <c r="C150" t="s">
+        <v>134</v>
+      </c>
+      <c r="D150">
+        <v>240</v>
+      </c>
+      <c r="E150" t="s">
+        <v>208</v>
+      </c>
+      <c r="F150">
+        <v>1968</v>
+      </c>
+      <c r="G150">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>19</v>
+      </c>
+      <c r="B151" t="s">
+        <v>72</v>
+      </c>
+      <c r="C151" t="s">
+        <v>135</v>
+      </c>
+      <c r="D151">
+        <v>4000</v>
+      </c>
+      <c r="E151" t="s">
+        <v>209</v>
+      </c>
+      <c r="F151">
+        <v>77312</v>
+      </c>
+      <c r="G151">
+        <v>12.92</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>19</v>
+      </c>
+      <c r="B152" t="s">
+        <v>72</v>
+      </c>
+      <c r="C152" t="s">
+        <v>136</v>
+      </c>
+      <c r="D152">
+        <v>25000</v>
+      </c>
+      <c r="E152" t="s">
+        <v>210</v>
+      </c>
+      <c r="F152">
+        <v>474125</v>
+      </c>
+      <c r="G152">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>19</v>
+      </c>
+      <c r="B153" t="s">
+        <v>73</v>
+      </c>
+      <c r="C153" t="s">
+        <v>136</v>
+      </c>
+      <c r="D153">
+        <v>25000</v>
+      </c>
+      <c r="E153" t="s">
+        <v>211</v>
+      </c>
+      <c r="F153">
+        <v>628377.5</v>
+      </c>
+      <c r="G153">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>20</v>
+      </c>
+      <c r="B154" t="s">
+        <v>74</v>
+      </c>
+      <c r="C154" t="s">
+        <v>137</v>
+      </c>
+      <c r="D154">
+        <v>1000</v>
+      </c>
+      <c r="E154" t="s">
+        <v>212</v>
+      </c>
+      <c r="F154">
+        <v>143930</v>
+      </c>
+      <c r="G154">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>20</v>
+      </c>
+      <c r="B155" t="s">
+        <v>75</v>
+      </c>
+      <c r="C155" t="s">
+        <v>137</v>
+      </c>
+      <c r="D155">
+        <v>1000</v>
+      </c>
+      <c r="E155" t="s">
+        <v>213</v>
+      </c>
+      <c r="F155">
+        <v>149270</v>
+      </c>
+      <c r="G155">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>20</v>
+      </c>
+      <c r="B156" t="s">
+        <v>76</v>
+      </c>
+      <c r="C156" t="s">
+        <v>138</v>
+      </c>
+      <c r="D156">
+        <v>1000</v>
+      </c>
+      <c r="E156" t="s">
+        <v>214</v>
+      </c>
+      <c r="F156">
+        <v>132870</v>
+      </c>
+      <c r="G156">
+        <v>1538.46</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>21</v>
+      </c>
+      <c r="B157" t="s">
+        <v>77</v>
+      </c>
+      <c r="C157" t="s">
+        <v>139</v>
+      </c>
+      <c r="D157">
+        <v>6.9116</v>
+      </c>
+      <c r="E157" t="s">
+        <v>215</v>
+      </c>
+      <c r="F157">
+        <v>517.60350356</v>
+      </c>
+      <c r="G157">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>21</v>
+      </c>
+      <c r="B158" t="s">
+        <v>78</v>
+      </c>
+      <c r="C158" t="s">
+        <v>139</v>
+      </c>
+      <c r="D158">
+        <v>659</v>
+      </c>
+      <c r="E158" t="s">
+        <v>216</v>
+      </c>
+      <c r="F158">
+        <v>49682.01</v>
+      </c>
+      <c r="G158">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>21</v>
+      </c>
+      <c r="B159" t="s">
+        <v>79</v>
+      </c>
+      <c r="C159" t="s">
+        <v>140</v>
+      </c>
+      <c r="D159">
+        <v>625000</v>
+      </c>
+      <c r="E159" t="s">
+        <v>217</v>
+      </c>
+      <c r="F159">
+        <v>10000000</v>
+      </c>
+      <c r="G159">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>21</v>
+      </c>
+      <c r="B160" t="s">
+        <v>80</v>
+      </c>
+      <c r="C160" t="s">
+        <v>141</v>
+      </c>
+      <c r="D160">
+        <v>20000</v>
+      </c>
+      <c r="E160" t="s">
+        <v>218</v>
+      </c>
+      <c r="F160">
+        <v>481965.9999999999</v>
+      </c>
+      <c r="G160">
+        <v>133.33</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>22</v>
+      </c>
+      <c r="B161" t="s">
+        <v>69</v>
+      </c>
+      <c r="C161" t="s">
+        <v>142</v>
+      </c>
+      <c r="D161">
+        <v>3786</v>
+      </c>
+      <c r="E161" t="s">
+        <v>219</v>
+      </c>
+      <c r="F161">
+        <v>492937.2</v>
+      </c>
+      <c r="G161">
+        <v>103.08</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>22</v>
+      </c>
+      <c r="B162" t="s">
+        <v>81</v>
+      </c>
+      <c r="C162" t="s">
+        <v>143</v>
+      </c>
+      <c r="D162">
+        <v>56</v>
+      </c>
+      <c r="E162" t="s">
+        <v>220</v>
+      </c>
+      <c r="F162">
+        <v>7899.92</v>
+      </c>
+      <c r="G162">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163" t="s">
+        <v>82</v>
+      </c>
+      <c r="C163" t="s">
+        <v>142</v>
+      </c>
+      <c r="D163">
+        <v>1400</v>
+      </c>
+      <c r="E163" t="s">
+        <v>221</v>
+      </c>
+      <c r="F163">
+        <v>199290</v>
+      </c>
+      <c r="G163">
+        <v>61.59</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" t="s">
+        <v>22</v>
+      </c>
+      <c r="B164" t="s">
+        <v>83</v>
+      </c>
+      <c r="C164" t="s">
+        <v>142</v>
+      </c>
+      <c r="D164">
+        <v>675</v>
+      </c>
+      <c r="E164" t="s">
+        <v>222</v>
+      </c>
+      <c r="F164">
+        <v>98475.74999999999</v>
+      </c>
+      <c r="G164">
+        <v>119.89</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" t="s">
+        <v>22</v>
+      </c>
+      <c r="B165" t="s">
+        <v>84</v>
+      </c>
+      <c r="C165" t="s">
+        <v>143</v>
+      </c>
+      <c r="D165">
+        <v>61</v>
+      </c>
+      <c r="E165" t="s">
+        <v>223</v>
+      </c>
+      <c r="F165">
+        <v>8834.630000000001</v>
+      </c>
+      <c r="G165">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>22</v>
+      </c>
+      <c r="B166" t="s">
+        <v>85</v>
+      </c>
+      <c r="C166" t="s">
+        <v>144</v>
+      </c>
+      <c r="D166">
+        <v>2000</v>
+      </c>
+      <c r="E166" t="s">
+        <v>224</v>
+      </c>
+      <c r="F166">
+        <v>231900</v>
+      </c>
+      <c r="G166">
+        <v>48.78</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>23</v>
+      </c>
+      <c r="B167" t="s">
+        <v>86</v>
+      </c>
+      <c r="C167" t="s">
+        <v>145</v>
+      </c>
+      <c r="D167">
+        <v>1764705</v>
+      </c>
+      <c r="E167" t="s">
+        <v>225</v>
+      </c>
+      <c r="F167">
+        <v>29999985</v>
+      </c>
+      <c r="G167">
+        <v>5.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>